<commit_message>
Criação do caso de testes - Abrir e Fechar Semestre
O caso de uso foi criado, faltando apenas ser passado para o template
correto.
</commit_message>
<xml_diff>
--- a/casos de testes/UC - Alocar professor a uma disciplina.xlsx
+++ b/casos de testes/UC - Alocar professor a uma disciplina.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>UC001 - Alocar Professor em uma Disciplina</t>
   </si>
@@ -124,6 +124,63 @@
   </si>
   <si>
     <t>UC001 - Abrir e fechar semestre</t>
+  </si>
+  <si>
+    <t>Clicar no botão "Fechar" localizado ao lado do período para fechamento do semestre atual.</t>
+  </si>
+  <si>
+    <t>O status do semestre atual ficará igua a "Fechado".</t>
+  </si>
+  <si>
+    <t>Clicar no botão "Fechar trabalho" ao lado de todos os trabalhos do semestre atual que estão com status de aberto.</t>
+  </si>
+  <si>
+    <t>Todos ostrabalhos referentes ao semestre atual serão fechados com sucesso.</t>
+  </si>
+  <si>
+    <t>Verificar no banco de dados o relacionamento entre os envolvidos do semestre atual</t>
+  </si>
+  <si>
+    <t>Todos os relacionamentos deverão ser desfietos</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Adicionar novo semestre".</t>
+  </si>
+  <si>
+    <t>O sistema carrega a página informando os campos para preenchimento dos dados do novo semestre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preencher todos os campos obrigatórios e clicar em "Cadastrar" </t>
+  </si>
+  <si>
+    <t>O sistema exibe uma mensagem informando que o semestre foi cadastrado com sucesso.</t>
+  </si>
+  <si>
+    <t>Verificar o status do novo semestre</t>
+  </si>
+  <si>
+    <t>Após a criação do novo semestre, seu status deverá ser igual a "atual"</t>
+  </si>
+  <si>
+    <t>Fluxo de Exceção</t>
+  </si>
+  <si>
+    <t>Preencher o campo "Ano do semestre" do novo semestre menor  que o ano do semestre que foi fechado</t>
+  </si>
+  <si>
+    <t>Uma mensagem de erro deverá ser mostrada afirmando que não é possível criar um novo semestre com ano menor que o semestre anterior. O cadastro é cancelado.</t>
+  </si>
+  <si>
+    <t>Preencher os campos sem preencher os campos obrigatórios</t>
+  </si>
+  <si>
+    <t>Uma mensagem de erro será mostrada informando que os campos obrigatórios deverão ser preenchido. Voltar pra tela de preenchimento dos campos</t>
+  </si>
+  <si>
+    <t>Cadastrar um semestre já existente</t>
+  </si>
+  <si>
+    <t>Uma mensagem de erro será mostrada informando que o semestre já existe. O cadastro é cancelado.</t>
   </si>
 </sst>
 </file>
@@ -201,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +282,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -689,8 +753,110 @@
         <v>3</v>
       </c>
     </row>
+    <row r="17" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A9:C9"/>

</xml_diff>